<commit_message>
ajout zones de déplacement ennemis sur la gamemap
</commit_message>
<xml_diff>
--- a/GameMap Schema.xlsx
+++ b/GameMap Schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e73f471c775c8904/Sauvegarde PC-STDO/Desktop/Documents/Clément/Matières/NSI/Python/Projets/SpaceInvaders/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7120EC7D-99E2-4DE6-9933-A0094F7827AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{7120EC7D-99E2-4DE6-9933-A0094F7827AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8DE7A0E8-CE2E-4528-9774-915614ACA01B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3CCF9B41-BC7F-4DC3-BF66-4C463633BC9E}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>: rien (barrière à la fin éventuellement)</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t xml:space="preserve"> : ennemi = carré de 100 par 100</t>
+  </si>
+  <si>
+    <t>: zone de mouvement des ennemis</t>
   </si>
 </sst>
 </file>
@@ -69,7 +72,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -100,6 +103,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="lightGrid">
+        <bgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="6">
     <border>
@@ -172,55 +180,56 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -538,7 +547,7 @@
   <dimension ref="B2:S15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S4" sqref="S4"/>
+      <selection activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,252 +556,275 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:19" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="14"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="5"/>
     </row>
     <row r="3" spans="2:19" ht="48" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="13"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="13"/>
-      <c r="R3" s="6"/>
-      <c r="S3" s="5" t="s">
+      <c r="B3" s="22"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="22"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="2:19" ht="48" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="13"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="13"/>
-      <c r="R4" s="19"/>
-      <c r="S4" s="5" t="s">
+      <c r="B4" s="22"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="22"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:19" ht="48" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B5" s="13"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="13"/>
-      <c r="R5" s="12"/>
-      <c r="S5" s="5" t="s">
+      <c r="B5" s="22"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="19"/>
+      <c r="O5" s="22"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:19" ht="48" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="13"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="13"/>
-      <c r="R6" s="20"/>
-      <c r="S6" s="21" t="s">
+      <c r="B6" s="22"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="21"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="21"/>
+      <c r="O6" s="22"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:19" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="13"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="13"/>
+    <row r="7" spans="2:19" ht="48" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B7" s="22"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="19"/>
+      <c r="O7" s="22"/>
+      <c r="R7" s="22"/>
+      <c r="S7" s="8" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="8" spans="2:19" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="13"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="13"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="22"/>
     </row>
     <row r="9" spans="2:19" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="13"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="13"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="19"/>
+      <c r="O9" s="22"/>
     </row>
     <row r="10" spans="2:19" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="13"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="13"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="21"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="21"/>
+      <c r="O10" s="22"/>
     </row>
     <row r="11" spans="2:19" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="13"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="16"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="16"/>
-      <c r="O11" s="13"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="4"/>
     </row>
     <row r="12" spans="2:19" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="13"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="18"/>
-      <c r="M12" s="17"/>
-      <c r="N12" s="18"/>
-      <c r="O12" s="13"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="17"/>
+      <c r="O12" s="4"/>
     </row>
     <row r="13" spans="2:19" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="13"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="13"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="4"/>
     </row>
     <row r="14" spans="2:19" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="13"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="7"/>
-      <c r="O14" s="13"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="4"/>
     </row>
     <row r="15" spans="2:19" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="13"/>
-      <c r="N15" s="13"/>
-      <c r="O15" s="13"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="C13:D14"/>
-    <mergeCell ref="E13:F14"/>
-    <mergeCell ref="G13:H14"/>
-    <mergeCell ref="I13:J14"/>
-    <mergeCell ref="K13:L14"/>
+    <mergeCell ref="M5:N6"/>
+    <mergeCell ref="C3:D4"/>
+    <mergeCell ref="E3:F4"/>
+    <mergeCell ref="G3:H4"/>
+    <mergeCell ref="I3:J4"/>
+    <mergeCell ref="K3:L4"/>
+    <mergeCell ref="M3:N4"/>
+    <mergeCell ref="C5:D6"/>
+    <mergeCell ref="E5:F6"/>
+    <mergeCell ref="G5:H6"/>
+    <mergeCell ref="I5:J6"/>
+    <mergeCell ref="K5:L6"/>
+    <mergeCell ref="M9:N10"/>
+    <mergeCell ref="C7:D8"/>
+    <mergeCell ref="E7:F8"/>
+    <mergeCell ref="G7:H8"/>
+    <mergeCell ref="I7:J8"/>
+    <mergeCell ref="K7:L8"/>
+    <mergeCell ref="M7:N8"/>
+    <mergeCell ref="C9:D10"/>
+    <mergeCell ref="E9:F10"/>
+    <mergeCell ref="G9:H10"/>
+    <mergeCell ref="I9:J10"/>
+    <mergeCell ref="K9:L10"/>
     <mergeCell ref="M13:N14"/>
     <mergeCell ref="C11:D12"/>
     <mergeCell ref="E11:F12"/>
@@ -800,30 +832,11 @@
     <mergeCell ref="I11:J12"/>
     <mergeCell ref="K11:L12"/>
     <mergeCell ref="M11:N12"/>
-    <mergeCell ref="C9:D10"/>
-    <mergeCell ref="E9:F10"/>
-    <mergeCell ref="G9:H10"/>
-    <mergeCell ref="I9:J10"/>
-    <mergeCell ref="K9:L10"/>
-    <mergeCell ref="M9:N10"/>
-    <mergeCell ref="C7:D8"/>
-    <mergeCell ref="E7:F8"/>
-    <mergeCell ref="G7:H8"/>
-    <mergeCell ref="I7:J8"/>
-    <mergeCell ref="K7:L8"/>
-    <mergeCell ref="M7:N8"/>
-    <mergeCell ref="C5:D6"/>
-    <mergeCell ref="E5:F6"/>
-    <mergeCell ref="G5:H6"/>
-    <mergeCell ref="I5:J6"/>
-    <mergeCell ref="K5:L6"/>
-    <mergeCell ref="M5:N6"/>
-    <mergeCell ref="C3:D4"/>
-    <mergeCell ref="E3:F4"/>
-    <mergeCell ref="G3:H4"/>
-    <mergeCell ref="I3:J4"/>
-    <mergeCell ref="K3:L4"/>
-    <mergeCell ref="M3:N4"/>
+    <mergeCell ref="C13:D14"/>
+    <mergeCell ref="E13:F14"/>
+    <mergeCell ref="G13:H14"/>
+    <mergeCell ref="I13:J14"/>
+    <mergeCell ref="K13:L14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>